<commit_message>
Automatically add new CCTV to DB
get online cctv list, scrape only online cctv, store the new cctc in DB, GUI update
</commit_message>
<xml_diff>
--- a/Data/cctv_locations_master.xlsx
+++ b/Data/cctv_locations_master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naris\Desktop\STIU\2024-1 Internship\Gistda\2024-07-01 Image Scraping\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917C4CBD-2519-4CAF-A5F6-F564C39CBACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CD61DA-7698-43A4-9EEB-A2E620EA042F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6575" uniqueCount="4083">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6613" uniqueCount="4101">
   <si>
     <t>ID</t>
   </si>
@@ -12282,6 +12282,60 @@
   </si>
   <si>
     <t>Ratchawithi Intersection (Ratchawithi Road Side)</t>
+  </si>
+  <si>
+    <t>1286</t>
+  </si>
+  <si>
+    <t>TF1-BA-03</t>
+  </si>
+  <si>
+    <t>ถ.สุขาภิบาล 5 ตัด ซ.32 วัชรพล</t>
+  </si>
+  <si>
+    <t>10.156.101.55</t>
+  </si>
+  <si>
+    <t>1293</t>
+  </si>
+  <si>
+    <t>TF1-NK-02</t>
+  </si>
+  <si>
+    <t>แยกเพชรเกษม 81</t>
+  </si>
+  <si>
+    <t>10.156.101.9</t>
+  </si>
+  <si>
+    <t>1327</t>
+  </si>
+  <si>
+    <t>TF1-TW-04</t>
+  </si>
+  <si>
+    <t>ถ.เพชรเกษม ตัด ถ.ทวีวัฒนา</t>
+  </si>
+  <si>
+    <t>10.156.101.1</t>
+  </si>
+  <si>
+    <t>1692</t>
+  </si>
+  <si>
+    <t>ถ.บรมราชชนนี ตัด ถ.ราชพฤกษ์</t>
+  </si>
+  <si>
+    <t>10.156.101.14</t>
+  </si>
+  <si>
+    <t>1744</t>
+  </si>
+  <si>
+    <t>แยกบางบอน 5</t>
+  </si>
+  <si>
+    <t>10.150.101.56</t>
   </si>
 </sst>
 </file>
@@ -12696,11 +12750,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M689"/>
+  <dimension ref="A1:M694"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A380" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J402" sqref="J402"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A587" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E696" sqref="E696"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -37967,7 +38021,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="689" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="689" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A689" t="s">
         <v>3941</v>
       </c>
@@ -37993,6 +38047,160 @@
         <v>3943</v>
       </c>
       <c r="J689" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="690" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A690" t="s">
+        <v>4083</v>
+      </c>
+      <c r="B690" t="s">
+        <v>4084</v>
+      </c>
+      <c r="D690" t="s">
+        <v>4085</v>
+      </c>
+      <c r="E690" t="s">
+        <v>9</v>
+      </c>
+      <c r="F690" t="s">
+        <v>4085</v>
+      </c>
+      <c r="G690" t="s">
+        <v>9</v>
+      </c>
+      <c r="H690">
+        <v>13.884600000000001</v>
+      </c>
+      <c r="I690">
+        <v>100.65362</v>
+      </c>
+      <c r="L690" t="s">
+        <v>4086</v>
+      </c>
+      <c r="M690" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="691" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A691" t="s">
+        <v>4087</v>
+      </c>
+      <c r="B691" t="s">
+        <v>4088</v>
+      </c>
+      <c r="D691" t="s">
+        <v>4089</v>
+      </c>
+      <c r="E691" t="s">
+        <v>9</v>
+      </c>
+      <c r="F691" t="s">
+        <v>4089</v>
+      </c>
+      <c r="G691" t="s">
+        <v>9</v>
+      </c>
+      <c r="H691">
+        <v>13.70565</v>
+      </c>
+      <c r="I691">
+        <v>100.3433</v>
+      </c>
+      <c r="L691" t="s">
+        <v>4090</v>
+      </c>
+      <c r="M691" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="692" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A692" t="s">
+        <v>4091</v>
+      </c>
+      <c r="B692" t="s">
+        <v>4092</v>
+      </c>
+      <c r="D692" t="s">
+        <v>4093</v>
+      </c>
+      <c r="E692" t="s">
+        <v>9</v>
+      </c>
+      <c r="F692" t="s">
+        <v>4093</v>
+      </c>
+      <c r="G692" t="s">
+        <v>9</v>
+      </c>
+      <c r="H692">
+        <v>13.70806</v>
+      </c>
+      <c r="I692">
+        <v>100.37348</v>
+      </c>
+      <c r="L692" t="s">
+        <v>4094</v>
+      </c>
+      <c r="M692" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="693" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A693" t="s">
+        <v>4095</v>
+      </c>
+      <c r="D693" t="s">
+        <v>4096</v>
+      </c>
+      <c r="E693" t="s">
+        <v>9</v>
+      </c>
+      <c r="F693" t="s">
+        <v>9</v>
+      </c>
+      <c r="G693" t="s">
+        <v>9</v>
+      </c>
+      <c r="H693">
+        <v>13.779949999999999</v>
+      </c>
+      <c r="I693">
+        <v>100.44307999999999</v>
+      </c>
+      <c r="L693" t="s">
+        <v>4097</v>
+      </c>
+      <c r="M693" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="694" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A694" t="s">
+        <v>4098</v>
+      </c>
+      <c r="D694" t="s">
+        <v>4099</v>
+      </c>
+      <c r="E694" t="s">
+        <v>9</v>
+      </c>
+      <c r="F694" t="s">
+        <v>9</v>
+      </c>
+      <c r="G694" t="s">
+        <v>9</v>
+      </c>
+      <c r="H694">
+        <v>13.63851</v>
+      </c>
+      <c r="I694">
+        <v>100.37191</v>
+      </c>
+      <c r="L694" t="s">
+        <v>4100</v>
+      </c>
+      <c r="M694" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto CCTV update and clustering
The script will now check for online cameras on the server and update the database with any new cameras, including auto-clustering for all cameras. Additionally, it will only attempt to scrape images from currently online CCTV cameras.
</commit_message>
<xml_diff>
--- a/Data/cctv_locations_master.xlsx
+++ b/Data/cctv_locations_master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naris\Desktop\STIU\2024-1 Internship\Gistda\2024-07-01 Image Scraping\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CD61DA-7698-43A4-9EEB-A2E620EA042F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F91AF03-628D-4D4A-A7B6-2399EE165EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6613" uniqueCount="4101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6648" uniqueCount="4119">
   <si>
     <t>ID</t>
   </si>
@@ -12336,6 +12336,60 @@
   </si>
   <si>
     <t>10.150.101.56</t>
+  </si>
+  <si>
+    <t>1098</t>
+  </si>
+  <si>
+    <t>ถนนบรมราชชนนี ตัด ถนนพุทธมณฑลสาย 1</t>
+  </si>
+  <si>
+    <t>Thanon Phutthamonthon Sal 1</t>
+  </si>
+  <si>
+    <t>10.156.101.25</t>
+  </si>
+  <si>
+    <t>1774</t>
+  </si>
+  <si>
+    <t>แยกบางนา</t>
+  </si>
+  <si>
+    <t>รถมุ่งหน้าศรีนครินทร์</t>
+  </si>
+  <si>
+    <t>10.156.102.34</t>
+  </si>
+  <si>
+    <t>1776</t>
+  </si>
+  <si>
+    <t>สะพานควาย</t>
+  </si>
+  <si>
+    <t>สะพานลอยแยกสะพานควาย</t>
+  </si>
+  <si>
+    <t>10.114.101.3</t>
+  </si>
+  <si>
+    <t>242</t>
+  </si>
+  <si>
+    <t>10.107.129.130</t>
+  </si>
+  <si>
+    <t>1775</t>
+  </si>
+  <si>
+    <t>อุโมงค์ทางลอดพระราม 9</t>
+  </si>
+  <si>
+    <t>รถมุ่งหน้ารามคำแหง</t>
+  </si>
+  <si>
+    <t>10.156.102.64</t>
   </si>
 </sst>
 </file>
@@ -12750,11 +12804,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M694"/>
+  <dimension ref="A1:M699"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A587" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E696" sqref="E696"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A683" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L695" sqref="L695:M699"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -38204,6 +38258,151 @@
         <v>11</v>
       </c>
     </row>
+    <row r="695" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A695" t="s">
+        <v>4101</v>
+      </c>
+      <c r="D695" t="s">
+        <v>4102</v>
+      </c>
+      <c r="E695" t="s">
+        <v>4103</v>
+      </c>
+      <c r="F695" t="s">
+        <v>4102</v>
+      </c>
+      <c r="G695" t="s">
+        <v>4103</v>
+      </c>
+      <c r="H695">
+        <v>13.780939999999999</v>
+      </c>
+      <c r="I695">
+        <v>100.42673000000001</v>
+      </c>
+      <c r="L695" t="s">
+        <v>4104</v>
+      </c>
+      <c r="M695" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="696" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A696" t="s">
+        <v>4105</v>
+      </c>
+      <c r="D696" t="s">
+        <v>4106</v>
+      </c>
+      <c r="E696" t="s">
+        <v>9</v>
+      </c>
+      <c r="F696" t="s">
+        <v>4107</v>
+      </c>
+      <c r="G696" t="s">
+        <v>9</v>
+      </c>
+      <c r="H696">
+        <v>13.67371</v>
+      </c>
+      <c r="I696">
+        <v>100.60714</v>
+      </c>
+      <c r="L696" t="s">
+        <v>4108</v>
+      </c>
+      <c r="M696" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="697" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A697" t="s">
+        <v>4109</v>
+      </c>
+      <c r="D697" t="s">
+        <v>4110</v>
+      </c>
+      <c r="E697" t="s">
+        <v>9</v>
+      </c>
+      <c r="F697" t="s">
+        <v>4111</v>
+      </c>
+      <c r="G697" t="s">
+        <v>9</v>
+      </c>
+      <c r="H697">
+        <v>13.78975</v>
+      </c>
+      <c r="I697">
+        <v>100.54824000000001</v>
+      </c>
+      <c r="L697" t="s">
+        <v>4112</v>
+      </c>
+      <c r="M697" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="698" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A698" t="s">
+        <v>4113</v>
+      </c>
+      <c r="D698" t="s">
+        <v>2083</v>
+      </c>
+      <c r="E698" t="s">
+        <v>9</v>
+      </c>
+      <c r="F698" t="s">
+        <v>2084</v>
+      </c>
+      <c r="G698" t="s">
+        <v>9</v>
+      </c>
+      <c r="H698">
+        <v>13.747299999999999</v>
+      </c>
+      <c r="I698">
+        <v>100.53082000000001</v>
+      </c>
+      <c r="L698" t="s">
+        <v>4114</v>
+      </c>
+      <c r="M698" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="699" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A699" t="s">
+        <v>4115</v>
+      </c>
+      <c r="D699" t="s">
+        <v>4116</v>
+      </c>
+      <c r="E699" t="s">
+        <v>9</v>
+      </c>
+      <c r="F699" t="s">
+        <v>4117</v>
+      </c>
+      <c r="G699" t="s">
+        <v>9</v>
+      </c>
+      <c r="H699">
+        <v>13.741960000000001</v>
+      </c>
+      <c r="I699">
+        <v>100.61592</v>
+      </c>
+      <c r="L699" t="s">
+        <v>4118</v>
+      </c>
+      <c r="M699" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>